<commit_message>
Updates to make data reading process cleaner and more accurate.
</commit_message>
<xml_diff>
--- a/nps_parks_master_df.xlsx
+++ b/nps_parks_master_df.xlsx
@@ -4444,7 +4444,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>coro</t>
+          <t>xxx1</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4452,17 +4452,9 @@
           <t>National Memorials</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>AZ</t>
-        </is>
-      </c>
-      <c r="F127" t="n">
-        <v>31.34900397</v>
-      </c>
-      <c r="G127" t="n">
-        <v>-110.2561574</v>
-      </c>
+      <c r="E127" t="inlineStr"/>
+      <c r="F127" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
       <c r="H127" t="inlineStr"/>
     </row>
     <row r="128">
@@ -7264,7 +7256,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>mabi</t>
+          <t>xxx2</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -7272,17 +7264,9 @@
           <t>National Parkways</t>
         </is>
       </c>
-      <c r="E214" t="inlineStr">
-        <is>
-          <t>VT</t>
-        </is>
-      </c>
-      <c r="F214" t="n">
-        <v>43.63348732</v>
-      </c>
-      <c r="G214" t="n">
-        <v>-72.53424638</v>
-      </c>
+      <c r="E214" t="inlineStr"/>
+      <c r="F214" t="inlineStr"/>
+      <c r="G214" t="inlineStr"/>
       <c r="H214" t="inlineStr"/>
     </row>
     <row r="215">
@@ -7950,7 +7934,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>lake</t>
+          <t>xxx3</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -7958,17 +7942,9 @@
           <t>National Recreation Areas</t>
         </is>
       </c>
-      <c r="E235" t="inlineStr">
-        <is>
-          <t>AZ,NV</t>
-        </is>
-      </c>
-      <c r="F235" t="n">
-        <v>35.96622528</v>
-      </c>
-      <c r="G235" t="n">
-        <v>-114.3469067</v>
-      </c>
+      <c r="E235" t="inlineStr"/>
+      <c r="F235" t="inlineStr"/>
+      <c r="G235" t="inlineStr"/>
       <c r="H235" t="inlineStr"/>
     </row>
     <row r="236">
@@ -8758,7 +8734,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>malu</t>
+          <t>mlkm</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -8768,14 +8744,14 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="F260" t="n">
-        <v>33.75618241</v>
+        <v>38.8862276865</v>
       </c>
       <c r="G260" t="n">
-        <v>-84.37256768</v>
+        <v>-77.0442195534</v>
       </c>
       <c r="H260" t="inlineStr"/>
     </row>
@@ -9984,7 +9960,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>jela</t>
+          <t>orca</t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
@@ -9994,14 +9970,14 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>LA</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="F298" t="n">
-        <v>29.81739855</v>
+        <v>42.10319143</v>
       </c>
       <c r="G298" t="n">
-        <v>-90.1402241</v>
+        <v>-123.4018586</v>
       </c>
       <c r="H298" t="inlineStr"/>
     </row>
@@ -11204,7 +11180,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>lake</t>
+          <t>xxx4</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
@@ -11212,17 +11188,9 @@
           <t>National Recreation Areas</t>
         </is>
       </c>
-      <c r="E336" t="inlineStr">
-        <is>
-          <t>AZ,NV</t>
-        </is>
-      </c>
-      <c r="F336" t="n">
-        <v>35.96622528</v>
-      </c>
-      <c r="G336" t="n">
-        <v>-114.3469067</v>
-      </c>
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="inlineStr"/>
+      <c r="G336" t="inlineStr"/>
       <c r="H336" t="inlineStr"/>
     </row>
     <row r="337">
@@ -12558,7 +12526,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>timu</t>
+          <t>nama</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
@@ -12568,14 +12536,14 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>FL</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="F378" t="n">
-        <v>30.47251894</v>
+        <v>38.88162683</v>
       </c>
       <c r="G378" t="n">
-        <v>-81.49950104</v>
+        <v>-77.03586953</v>
       </c>
       <c r="H378" t="inlineStr"/>
     </row>
@@ -13394,7 +13362,7 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>whsa</t>
+          <t>whho</t>
         </is>
       </c>
       <c r="D404" t="inlineStr">
@@ -13404,14 +13372,14 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="F404" t="n">
-        <v>32.77907858</v>
+        <v>38.89541886</v>
       </c>
       <c r="G404" t="n">
-        <v>-106.3333461</v>
+        <v>-77.03654147</v>
       </c>
       <c r="H404" t="inlineStr"/>
     </row>
@@ -13652,7 +13620,7 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>wwii</t>
+          <t>xxx6</t>
         </is>
       </c>
       <c r="D412" t="inlineStr">
@@ -13660,17 +13628,9 @@
           <t>National Memorials</t>
         </is>
       </c>
-      <c r="E412" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="F412" t="n">
-        <v>38.88923917</v>
-      </c>
-      <c r="G412" t="n">
-        <v>-77.0403759</v>
-      </c>
+      <c r="E412" t="inlineStr"/>
+      <c r="F412" t="inlineStr"/>
+      <c r="G412" t="inlineStr"/>
       <c r="H412" t="inlineStr"/>
     </row>
     <row r="413">

</xml_diff>